<commit_message>
health bars, score on screen, update
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tariq Ali\Documents\CSE360-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tareq\CSE360-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10550"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10548"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Create second player</t>
   </si>
   <si>
-    <t>Planned</t>
-  </si>
-  <si>
     <t>Player Shooting mechanics</t>
   </si>
   <si>
@@ -123,13 +120,19 @@
   </si>
   <si>
     <t>1 to 14</t>
+  </si>
+  <si>
+    <t>deleting old bullets</t>
+  </si>
+  <si>
+    <t>1 to 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,14 +148,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,12 +159,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -201,19 +192,12 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -221,23 +205,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -557,324 +546,342 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" customWidth="1"/>
-    <col min="2" max="2" width="50.54296875" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" customWidth="1"/>
-    <col min="4" max="4" width="39.54296875" customWidth="1"/>
-    <col min="5" max="5" width="19.6328125" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" customWidth="1"/>
+    <col min="2" max="2" width="50.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="39.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="11">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="13">
+        <v>2</v>
+      </c>
+      <c r="E4" s="13"/>
+      <c r="F4" s="4">
+        <v>42461</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="11">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="13">
+        <v>3</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="11">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13">
+        <v>4</v>
+      </c>
+      <c r="E6" s="13">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="11">
+        <v>4</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="13">
+        <v>5</v>
+      </c>
+      <c r="E7" s="13">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>42468</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="11">
+        <v>5</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="13">
+        <v>5</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11">
+        <v>6</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="13">
+        <v>5</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11">
+        <v>7</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="13">
+        <v>5</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="4">
+        <v>42475</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="11">
+        <v>9</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="13">
+        <v>3</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="11">
+        <v>10</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="C13" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="13">
+        <v>2</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="11">
+        <v>11</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="11">
+        <v>12</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="13">
+        <v>3</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="4">
+        <v>42482</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="11">
+        <v>13</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="13">
+        <v>2</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7">
+        <v>15</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="9">
+        <v>2</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="7">
         <v>16</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="6">
-        <v>2</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7">
-        <v>42461</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="6">
-        <v>3</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6">
-        <v>4</v>
-      </c>
-      <c r="E6" s="6">
-        <v>2</v>
-      </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4">
-        <v>4</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6">
-        <v>5</v>
-      </c>
-      <c r="E7" s="6">
-        <v>2</v>
-      </c>
-      <c r="F7" s="7">
-        <v>42468</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="8">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="3">
-        <v>5</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="4">
-        <v>6</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="6">
-        <v>5</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="4">
-        <v>7</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="6">
-        <v>5</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="9"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="4">
-        <v>8</v>
-      </c>
-      <c r="B11" s="10" t="s">
+      <c r="B19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="9">
+        <v>2</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
         <v>12</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="6">
-        <v>4</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="7">
-        <v>42475</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="12">
-        <v>9</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="3">
-        <v>3</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="4">
-        <v>10</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="10">
-        <v>2</v>
-      </c>
-      <c r="D13" s="6">
-        <v>2</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="4">
-        <v>11</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="6">
-        <v>1</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="8">
-        <v>12</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="3">
-        <v>3</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="7">
-        <v>42482</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="8">
-        <v>13</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="3">
-        <v>2</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="8">
-        <v>14</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="3">
-        <v>2</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="8">
-        <v>15</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="3">
-        <v>2</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="9"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed the wall between the players, score is not yet saved after closing the game
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Ongoing</t>
-  </si>
-  <si>
     <t>Come up with three rules</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>Showing the winner</t>
   </si>
   <si>
-    <t>Deciding which of the two players gets to play first</t>
-  </si>
-  <si>
     <t>Create user interface</t>
   </si>
   <si>
@@ -114,9 +108,6 @@
   </si>
   <si>
     <t>2,3,4,5,6,7,11</t>
-  </si>
-  <si>
-    <t>1,2,3,4,6,7</t>
   </si>
   <si>
     <t>1 to 14</t>
@@ -190,24 +181,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -227,6 +206,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -545,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,12 +548,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -578,310 +566,293 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9">
+        <v>2</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="11">
+        <v>42461</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="9">
+        <v>3</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="9">
+        <v>4</v>
+      </c>
+      <c r="E6" s="9">
+        <v>2</v>
+      </c>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="9">
+        <v>5</v>
+      </c>
+      <c r="E7" s="9">
+        <v>2</v>
+      </c>
+      <c r="F7" s="11">
+        <v>42468</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9">
+        <v>5</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="9">
+        <v>5</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7">
+        <v>7</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="9">
+        <v>5</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5">
+        <v>4</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="11">
+        <v>42475</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7">
+        <v>9</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="9">
+        <v>3</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7">
+        <v>10</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="11">
+      <c r="C13" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="9">
+        <v>2</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7">
+        <v>11</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="9">
         <v>1</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="13">
+      <c r="E14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7">
+        <v>12</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="9">
+        <v>3</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="11">
+        <v>42482</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7">
+        <v>13</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="9">
         <v>2</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="4">
-        <v>42461</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="11">
-        <v>2</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="13">
-        <v>3</v>
-      </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="11">
-        <v>3</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="13">
-        <v>4</v>
-      </c>
-      <c r="E6" s="13">
-        <v>2</v>
-      </c>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="11">
-        <v>4</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="13">
-        <v>5</v>
-      </c>
-      <c r="E7" s="13">
-        <v>2</v>
-      </c>
-      <c r="F7" s="4">
-        <v>42468</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="11">
-        <v>5</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="13">
-        <v>5</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="11">
-        <v>6</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="13">
-        <v>5</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="11">
-        <v>7</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="13">
-        <v>5</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="E16" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="4">
-        <v>42475</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="11">
-        <v>9</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="13">
-        <v>3</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11">
-        <v>10</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="13">
-        <v>2</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="11">
-        <v>11</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="13">
-        <v>1</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11">
-        <v>12</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="13">
-        <v>3</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="4">
-        <v>42482</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="11">
-        <v>13</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="13">
-        <v>2</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
-        <v>14</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="5">
         <v>2</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="5">
+        <v>2</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="7">
-        <v>15</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="9">
-        <v>2</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="7">
-        <v>16</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="9">
-        <v>2</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a task in the backlog
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>1 to 4</t>
+  </si>
+  <si>
+    <t>saving the score in a file</t>
   </si>
 </sst>
 </file>
@@ -153,7 +156,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -176,12 +179,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -214,6 +228,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -534,7 +558,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -849,7 +873,26 @@
       </c>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
+        <v>17</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="16">
+        <v>2</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="17">
+        <v>42489</v>
+      </c>
+    </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>11</v>

</xml_diff>